<commit_message>
Fixing issue with Tetrabromobisphenol A not being including as carcinogen
</commit_message>
<xml_diff>
--- a/data/TSCA Fenceline Map Chem Hazard Data Extraction.xlsx
+++ b/data/TSCA Fenceline Map Chem Hazard Data Extraction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://edforg.sharepoint.com/sites/SaferChemicals-TSCA/Shared Documents/TSCA/TSCA Fenceline Map Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\OCE Dropbox\Jeremy Proville\EDF\TSCA Mapping\TSCA Data Analysis\R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3890BC9D-E3A5-4607-AA16-34197C0F7F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A26446-D2C8-44DF-BDBA-32529D4D8881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{7FEFC3C9-9C83-49AD-90A9-4B598C07F3FD}"/>
+    <workbookView xWindow="-26580" yWindow="4635" windowWidth="23040" windowHeight="12210" activeTab="2" xr2:uid="{7FEFC3C9-9C83-49AD-90A9-4B598C07F3FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete data" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="196">
   <si>
     <t>Carcinogens (15)</t>
   </si>
@@ -699,12 +699,15 @@
   <si>
     <t>*hazard score based off 2014 TSCA Work Plan Methods Document</t>
   </si>
+  <si>
+    <t>Tetrabromobisphenol A</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1307,26 +1310,26 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="72.85546875" style="1" customWidth="1"/>
-    <col min="2" max="3" width="8.7109375" style="1"/>
-    <col min="4" max="4" width="11.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.28515625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="72.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="72.88671875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="8.6640625" style="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="72.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" style="1" customWidth="1"/>
     <col min="13" max="13" width="19" style="1" customWidth="1"/>
     <col min="14" max="14" width="46" style="1" customWidth="1"/>
-    <col min="15" max="15" width="33.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.7109375" style="1"/>
+    <col min="15" max="15" width="33.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="39.6" customHeight="1">
+    <row r="1" spans="1:17" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34"/>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -1351,7 +1354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1395,7 +1398,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="29.1">
+    <row r="3" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -1439,7 +1442,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="29.1">
+    <row r="4" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -1483,7 +1486,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="29.1">
+    <row r="5" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -1527,7 +1530,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="29.1">
+    <row r="6" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1571,7 +1574,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
@@ -1615,7 +1618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="29.1">
+    <row r="8" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
@@ -1659,7 +1662,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1">
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>50</v>
       </c>
@@ -1706,7 +1709,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -1750,7 +1753,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="29.1">
+    <row r="11" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>57</v>
       </c>
@@ -1794,7 +1797,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="29.1">
+    <row r="12" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>60</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="29.1">
+    <row r="13" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>62</v>
       </c>
@@ -1873,7 +1876,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="72.599999999999994">
+    <row r="14" spans="1:17" ht="72" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>67</v>
       </c>
@@ -1922,7 +1925,7 @@
       <c r="P14" s="37"/>
       <c r="Q14" s="37"/>
     </row>
-    <row r="15" spans="1:17" ht="29.1">
+    <row r="15" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>74</v>
       </c>
@@ -1966,7 +1969,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="29.1">
+    <row r="16" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>76</v>
       </c>
@@ -2010,7 +2013,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>78</v>
       </c>
@@ -2054,7 +2057,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:15" hidden="1">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>82</v>
       </c>
@@ -2098,7 +2101,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="29.1">
+    <row r="19" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>85</v>
       </c>
@@ -2142,7 +2145,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>88</v>
       </c>
@@ -2186,7 +2189,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>91</v>
       </c>
@@ -2230,7 +2233,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>96</v>
       </c>
@@ -2274,7 +2277,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>101</v>
       </c>
@@ -2318,7 +2321,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="29.1">
+    <row r="24" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>106</v>
       </c>
@@ -2362,7 +2365,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="29.1">
+    <row r="25" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>110</v>
       </c>
@@ -2388,7 +2391,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>112</v>
       </c>
@@ -2432,7 +2435,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>116</v>
       </c>
@@ -2476,7 +2479,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>118</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="43.5">
+    <row r="29" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>122</v>
       </c>
@@ -2561,7 +2564,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="29.1">
+    <row r="30" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>126</v>
       </c>
@@ -2608,7 +2611,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>131</v>
       </c>
@@ -2652,7 +2655,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>134</v>
       </c>
@@ -2696,7 +2699,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>138</v>
       </c>
@@ -2740,7 +2743,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="34" spans="1:15" hidden="1">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>145</v>
       </c>
@@ -2784,7 +2787,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:15" hidden="1">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>148</v>
       </c>
@@ -2828,7 +2831,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:15" hidden="1">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>149</v>
       </c>
@@ -2872,7 +2875,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:15" hidden="1">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>151</v>
       </c>
@@ -2919,7 +2922,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:15" hidden="1">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>151</v>
       </c>
@@ -2966,7 +2969,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:15" hidden="1">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>151</v>
       </c>
@@ -3013,7 +3016,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:15" hidden="1">
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>151</v>
       </c>
@@ -3088,16 +3091,16 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" customWidth="1"/>
+    <col min="1" max="1" width="53.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
         <v>154</v>
       </c>
@@ -3111,7 +3114,7 @@
       </c>
       <c r="F1" s="38"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>157</v>
       </c>
@@ -3131,7 +3134,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>110</v>
       </c>
@@ -3151,7 +3154,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>67</v>
       </c>
@@ -3171,7 +3174,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>76</v>
       </c>
@@ -3191,7 +3194,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>106</v>
       </c>
@@ -3205,7 +3208,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>74</v>
       </c>
@@ -3219,7 +3222,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>62</v>
       </c>
@@ -3233,7 +3236,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -3250,7 +3253,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -3264,7 +3267,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -3278,7 +3281,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -3292,7 +3295,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>85</v>
       </c>
@@ -3306,7 +3309,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>96</v>
       </c>
@@ -3320,7 +3323,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -3328,7 +3331,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>57</v>
       </c>
@@ -3336,7 +3339,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
@@ -3344,15 +3347,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="1"/>
     </row>
@@ -3374,36 +3377,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C4E7569-6D29-4467-9597-E8DEEB24539B}">
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="12"/>
-    <col min="7" max="7" width="38.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="31.7109375" style="12" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="29" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="12" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="22" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" style="12" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="12"/>
-    <col min="15" max="15" width="38.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="12"/>
-    <col min="17" max="17" width="12.140625" style="12" customWidth="1"/>
-    <col min="18" max="18" width="29.7109375" style="13" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" style="13" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" style="12" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="12"/>
+    <col min="4" max="4" width="10.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="12"/>
+    <col min="7" max="7" width="38.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" style="12" customWidth="1"/>
+    <col min="9" max="9" width="31.6640625" style="12" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" style="29" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" style="12" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" style="22" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" style="12" customWidth="1"/>
+    <col min="14" max="14" width="9.109375" style="12"/>
+    <col min="15" max="15" width="38.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.109375" style="12"/>
+    <col min="17" max="17" width="12.109375" style="12" customWidth="1"/>
+    <col min="18" max="18" width="29.6640625" style="13" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" style="13" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" style="12" customWidth="1"/>
+    <col min="21" max="16384" width="9.109375" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>154</v>
       </c>
@@ -3425,7 +3428,7 @@
       <c r="T1" s="39"/>
       <c r="U1" s="39"/>
     </row>
-    <row r="2" spans="1:21" ht="29.1">
+    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>157</v>
       </c>
@@ -3482,7 +3485,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>110</v>
       </c>
@@ -3541,7 +3544,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="72.599999999999994">
+    <row r="4" spans="1:21" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>67</v>
       </c>
@@ -3600,7 +3603,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>76</v>
       </c>
@@ -3658,7 +3661,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>106</v>
       </c>
@@ -3694,7 +3697,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="43.5">
+    <row r="7" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>74</v>
       </c>
@@ -3737,7 +3740,7 @@
         <v>-0.46511627906976744</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>62</v>
       </c>
@@ -3773,7 +3776,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -3808,7 +3811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
@@ -3843,7 +3846,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -3879,7 +3882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -3914,7 +3917,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>85</v>
       </c>
@@ -3950,7 +3953,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>96</v>
       </c>
@@ -3986,7 +3989,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>42</v>
       </c>
@@ -4003,7 +4006,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>57</v>
       </c>
@@ -4023,7 +4026,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>60</v>
       </c>
@@ -4043,7 +4046,16 @@
         <v>193</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E18" s="12">
+        <v>0.8</v>
+      </c>
       <c r="G18" s="12" t="s">
         <v>194</v>
       </c>
@@ -4074,6 +4086,48 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="21d49585-c85a-4330-82bd-343b12f19e6c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="09c489fc-311a-4af8-8e4b-b0c8b19cb32b">
+      <UserInfo>
+        <DisplayName>Maria Doa</DisplayName>
+        <AccountId>10</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Paige Varner</DisplayName>
+        <AccountId>93</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jeremy Proville</DisplayName>
+        <AccountId>58</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Mary Collins</DisplayName>
+        <AccountId>57</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Liora Fiksel</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Lindsay McCormick</DisplayName>
+        <AccountId>12</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A753F85481C56F489ABD8D24FA5BAD7C" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f75fb1472f4308e77fd73d7909f109c2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="21d49585-c85a-4330-82bd-343b12f19e6c" xmlns:ns3="09c489fc-311a-4af8-8e4b-b0c8b19cb32b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="89beb3ea88f1d3c4c5d7761ff096975d" ns2:_="" ns3:_="">
     <xsd:import namespace="21d49585-c85a-4330-82bd-343b12f19e6c"/>
@@ -4266,56 +4320,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="21d49585-c85a-4330-82bd-343b12f19e6c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="09c489fc-311a-4af8-8e4b-b0c8b19cb32b">
-      <UserInfo>
-        <DisplayName>Maria Doa</DisplayName>
-        <AccountId>10</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Paige Varner</DisplayName>
-        <AccountId>93</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jeremy Proville</DisplayName>
-        <AccountId>58</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Mary Collins</DisplayName>
-        <AccountId>57</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Liora Fiksel</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Lindsay McCormick</DisplayName>
-        <AccountId>12</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE429576-8CC1-49EE-A264-F337992AE7F1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE429576-8CC1-49EE-A264-F337992AE7F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{729827FB-EB24-4A90-AD96-1C4F01085EC0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35B9AEB4-53E6-4A63-B946-62BDA9A992E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="21d49585-c85a-4330-82bd-343b12f19e6c"/>
+    <ds:schemaRef ds:uri="09c489fc-311a-4af8-8e4b-b0c8b19cb32b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35B9AEB4-53E6-4A63-B946-62BDA9A992E8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{729827FB-EB24-4A90-AD96-1C4F01085EC0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="21d49585-c85a-4330-82bd-343b12f19e6c"/>
+    <ds:schemaRef ds:uri="09c489fc-311a-4af8-8e4b-b0c8b19cb32b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>